<commit_message>
cleaning up data files
</commit_message>
<xml_diff>
--- a/InputFiles/1 Data-driven custom bag end-to-end completion/1-data.xlsx
+++ b/InputFiles/1 Data-driven custom bag end-to-end completion/1-data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="217">
   <si>
     <t>Order type</t>
   </si>
@@ -409,9 +409,6 @@
     <t>BPR</t>
   </si>
   <si>
-    <t>DDP</t>
-  </si>
-  <si>
     <t>PPC</t>
   </si>
   <si>
@@ -436,9 +433,6 @@
     <t xml:space="preserve">F00 </t>
   </si>
   <si>
-    <t>F01</t>
-  </si>
-  <si>
     <t>F02</t>
   </si>
   <si>
@@ -460,9 +454,6 @@
     <t>F08</t>
   </si>
   <si>
-    <t>FFP</t>
-  </si>
-  <si>
     <t>FS1</t>
   </si>
   <si>
@@ -541,12 +532,6 @@
     <t>TB7SX14SC-0</t>
   </si>
   <si>
-    <t>TA7ACDCC-061</t>
-  </si>
-  <si>
-    <t>TA6ESSP-0C</t>
-  </si>
-  <si>
     <t>TB7SX1SC</t>
   </si>
   <si>
@@ -607,9 +592,6 @@
     <t xml:space="preserve">A-NO </t>
   </si>
   <si>
-    <t>TA4ACSCUCC-01</t>
-  </si>
-  <si>
     <t>ConfigA2</t>
   </si>
   <si>
@@ -640,21 +622,9 @@
     <t>TB7SX7SC-016</t>
   </si>
   <si>
-    <t>TB6CT5CC</t>
-  </si>
-  <si>
-    <t>TB6CT5CC-06</t>
-  </si>
-  <si>
     <t>US00035015</t>
   </si>
   <si>
-    <t>TA5ACMFTWLC</t>
-  </si>
-  <si>
-    <t>TA6ESLBP-0C</t>
-  </si>
-  <si>
     <t>US00242885</t>
   </si>
   <si>
@@ -691,31 +661,10 @@
     <t>06Y USTPU25</t>
   </si>
   <si>
-    <t>06Y UST8TP1</t>
-  </si>
-  <si>
     <t>06Y UST8HSA</t>
   </si>
   <si>
-    <t>06Y UST8DEN</t>
-  </si>
-  <si>
     <t xml:space="preserve">06Y USTP </t>
-  </si>
-  <si>
-    <t>06Y ZC</t>
-  </si>
-  <si>
-    <t>TH7WEAMPBSC-P06</t>
-  </si>
-  <si>
-    <t>TA6ESSP</t>
-  </si>
-  <si>
-    <t>TA7ACDCC</t>
-  </si>
-  <si>
-    <t>TA5ACMFT</t>
   </si>
   <si>
     <t>TB7SXSF</t>
@@ -1735,7 +1684,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -1768,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AA2">
         <v>2</v>
@@ -1779,7 +1728,7 @@
         <v>99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>23</v>
@@ -1800,277 +1749,248 @@
         <v>1</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="AA3" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA4" s="4">
-        <v>2</v>
-      </c>
+    <row r="4" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>158</v>
+      <c r="J5" t="s">
+        <v>122</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>204</v>
+        <v>123</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="AA5" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="E7" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K6" s="4" t="s">
+      <c r="J7" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="X7" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="W6" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="X6" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AA6" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="Z7" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
-        <v>223</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA7" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="E8" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="J8" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="L8">
         <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AA8" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="E9" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="L9" s="4">
-        <v>1</v>
-      </c>
-      <c r="W9" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="Y9" s="4" t="s">
-        <v>161</v>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="AA9" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="L10" s="4">
+        <v>1</v>
+      </c>
+      <c r="W10" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="W10" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA11" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
+      <c r="A12" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AA12" s="4">
         <v>2</v>
@@ -2081,31 +2001,28 @@
         <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I13" s="4">
-        <v>2</v>
+        <v>137</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>160</v>
+        <v>199</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L13" s="4">
+        <v>200</v>
+      </c>
+      <c r="L13">
         <v>1</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AA13" s="4">
         <v>2</v>
@@ -2116,31 +2033,31 @@
         <v>22</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I14" s="4">
         <v>2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L14" s="4">
         <v>1</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA14" s="4">
         <v>2</v>
@@ -2151,31 +2068,31 @@
         <v>22</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I15" s="4">
         <v>2</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L15" s="4">
         <v>1</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA15" s="4">
         <v>2</v>
@@ -2186,99 +2103,99 @@
         <v>22</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I16" s="4">
         <v>2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L16" s="4">
         <v>1</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA16" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>209</v>
+      <c r="A17" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="I17" s="4"/>
+        <v>141</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2</v>
+      </c>
       <c r="J17" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L17" s="4">
         <v>1</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA17" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>22</v>
+      <c r="A18" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I18" s="4">
-        <v>2</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L18" s="4">
         <v>1</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA18" s="4">
         <v>2</v>
@@ -2289,31 +2206,31 @@
         <v>22</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I19" s="4">
         <v>2</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L19" s="4">
         <v>1</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA19" s="4">
         <v>2</v>
@@ -2321,31 +2238,34 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
+      </c>
+      <c r="I20" s="4">
+        <v>2</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L20" s="4">
         <v>1</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA20" s="4">
         <v>2</v>
@@ -2356,28 +2276,28 @@
         <v>99</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L21" s="4">
         <v>1</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA21" s="4">
         <v>2</v>
@@ -2388,28 +2308,28 @@
         <v>99</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L22" s="4">
         <v>1</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA22" s="4">
         <v>2</v>
@@ -2417,31 +2337,31 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L23" s="4">
         <v>1</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA23" s="4">
         <v>2</v>
@@ -2449,31 +2369,31 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L24" s="4">
         <v>1</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA24" s="4">
         <v>2</v>
@@ -2481,37 +2401,31 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L25" s="4">
         <v>1</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA25" s="4">
         <v>2</v>
@@ -2519,71 +2433,101 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>99</v>
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H26" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J26" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J26" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="K26" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L26" s="4">
+        <v>1</v>
+      </c>
+      <c r="W26" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA26" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L27" s="4">
         <v>8</v>
       </c>
-      <c r="W26" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA26" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="E27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="W27" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA27" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L28" s="4">
         <v>1</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA28" s="4">
         <v>2</v>
@@ -2591,31 +2535,31 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L29" s="4">
         <v>1</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA29" s="4">
         <v>2</v>
@@ -2623,31 +2567,31 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L30" s="4">
         <v>1</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA30" s="4">
         <v>2</v>
@@ -2655,31 +2599,31 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L31" s="4">
         <v>1</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA31" s="4">
         <v>2</v>
@@ -2687,31 +2631,31 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L32" s="4">
         <v>1</v>
       </c>
       <c r="W32" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA32" s="4">
         <v>2</v>
@@ -2719,31 +2663,31 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L33" s="4">
         <v>1</v>
       </c>
       <c r="W33" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA33" s="4">
         <v>2</v>
@@ -2751,31 +2695,31 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L34" s="4">
         <v>1</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA34" s="4">
         <v>2</v>
@@ -2783,31 +2727,31 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L35" s="4">
         <v>1</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA35" s="4">
         <v>2</v>
@@ -2821,155 +2765,76 @@
       <c r="K36" s="3"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I37">
-        <v>2</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="L37">
-        <v>1</v>
-      </c>
+      <c r="A37" s="5"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
       <c r="W37" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA37" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L38" s="4">
-        <v>1</v>
-      </c>
+      <c r="A38" s="5"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="4"/>
       <c r="W38" s="4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="AA38" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>149</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
       <c r="J39" s="3"/>
-      <c r="K39" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L39" s="4">
-        <v>1</v>
-      </c>
+      <c r="K39" s="3"/>
+      <c r="L39" s="4"/>
       <c r="W39" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="AA39" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L40" s="4">
-        <v>10</v>
-      </c>
+      <c r="A40" s="5"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="4"/>
       <c r="W40" s="1" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="AA40" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L41">
-        <v>1</v>
-      </c>
+      <c r="A41" s="5"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
       <c r="W41" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="X41" t="s">
         <v>125</v>
@@ -2979,26 +2844,9 @@
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" t="s">
-        <v>226</v>
-      </c>
-      <c r="F42" t="s">
-        <v>23</v>
-      </c>
-      <c r="J42" t="s">
-        <v>231</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L42">
-        <v>1</v>
-      </c>
+      <c r="A42" s="5"/>
       <c r="W42" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="X42" s="4" t="s">
         <v>127</v>
@@ -3008,29 +2856,12 @@
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" t="s">
-        <v>224</v>
-      </c>
-      <c r="F43" t="s">
-        <v>23</v>
-      </c>
-      <c r="I43">
-        <v>3</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L43" s="1">
-        <v>1</v>
-      </c>
+      <c r="A43" s="5"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="1"/>
       <c r="W43" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="X43" s="4" t="s">
         <v>125</v>
@@ -3040,171 +2871,88 @@
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F44" t="s">
-        <v>23</v>
-      </c>
+      <c r="A44" s="5"/>
+      <c r="E44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="4">
-        <v>7</v>
-      </c>
+      <c r="I44" s="4"/>
       <c r="J44" s="3"/>
-      <c r="K44" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L44" s="4">
-        <v>2</v>
-      </c>
+      <c r="K44" s="3"/>
+      <c r="L44" s="4"/>
       <c r="W44" s="4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="AA44">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="A45" s="5"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I45" s="4">
-        <v>7</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L45" s="4">
-        <v>1</v>
-      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="4"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="4"/>
       <c r="W45" s="4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="AA45">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" s="4">
-        <v>7</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L46">
-        <v>2</v>
-      </c>
+      <c r="A46" s="5"/>
+      <c r="E46" s="3"/>
+      <c r="I46" s="4"/>
+      <c r="K46" s="4"/>
       <c r="W46" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AA46">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="A47" s="5"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I47">
-        <v>7</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L47">
-        <v>1</v>
-      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="4"/>
+      <c r="K47" s="3"/>
       <c r="W47" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="AA47">
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I48" s="4">
-        <v>7</v>
-      </c>
-      <c r="K48" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="L48">
-        <v>1</v>
-      </c>
+      <c r="A48" s="5"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="K48" s="4"/>
       <c r="W48" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AA48">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I49" s="4">
-        <v>7</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L49">
-        <v>6</v>
-      </c>
+      <c r="A49" s="5"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="K49" s="3"/>
       <c r="W49" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="AA49">
         <v>3</v>
@@ -3427,7 +3175,7 @@
         <v>37</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="O1" t="s">
         <v>44</v>
@@ -3507,7 +3255,7 @@
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3593,7 +3341,7 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3667,7 +3415,7 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3703,7 +3451,7 @@
         <v>115</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AM4" s="1" t="s">
         <v>76</v>
@@ -3711,7 +3459,7 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -3728,7 +3476,7 @@
         <v>112</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>48</v>
@@ -3738,7 +3486,7 @@
         <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="M5" s="4">
         <v>423827</v>
@@ -3747,7 +3495,7 @@
         <v>38</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AM5" s="4" t="s">
         <v>76</v>
@@ -3755,7 +3503,7 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3775,7 +3523,7 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3790,7 +3538,7 @@
         <v>112</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>48</v>
@@ -3860,7 +3608,7 @@
         <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>32</v>
@@ -3899,7 +3647,7 @@
         <v>37</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>44</v>
@@ -3922,66 +3670,66 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>189</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H2" t="s">
         <v>112</v>
       </c>
       <c r="I2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="J2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="L2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="P2" t="s">
         <v>103</v>
       </c>
       <c r="Q2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="R2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="S2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="T2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -3989,71 +3737,71 @@
         <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="J3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="T3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F4">
         <v>423831</v>
       </c>
       <c r="G4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="T4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="U4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F5" s="4">
         <v>423844</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="U5" s="4"/>
     </row>

</xml_diff>